<commit_message>
New num of rounds table
</commit_message>
<xml_diff>
--- a/plots/Num of rounds.xlsx
+++ b/plots/Num of rounds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evana/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667A5A72-D443-1D41-AC46-F415371FE46A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605E0A63-CBE6-2F42-B1F2-6501E95566C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19380" activeTab="1" xr2:uid="{2E9F8102-5C57-5A42-8AAB-F246BFE78AC5}"/>
   </bookViews>
@@ -639,7 +639,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -980,7 +980,7 @@
     <cfRule type="dataBar" priority="2">
       <dataBar showValue="0">
         <cfvo type="min"/>
-        <cfvo type="num" val="300"/>
+        <cfvo type="max"/>
         <color theme="1" tint="0.249977111117893"/>
       </dataBar>
       <extLst>
@@ -1059,9 +1059,7 @@
           <x14:cfRule type="dataBar" id="{F9CD0769-6BAB-D042-B678-D8DF29716572}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="num">
-                <xm:f>300</xm:f>
-              </x14:cfvo>
+              <x14:cfvo type="autoMax"/>
               <x14:negativeFillColor rgb="FFFF0000"/>
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
@@ -1101,7 +1099,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1110,13 +1108,13 @@
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
     <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="8" max="8" width="16.83203125" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
-    <col min="11" max="11" width="16.83203125" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" customWidth="1"/>
     <col min="12" max="12" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1379,16 +1377,16 @@
     <row r="13" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="J6:K6"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="J6:K6"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E9">
     <cfRule type="dataBar" priority="6">
@@ -1436,7 +1434,7 @@
     <cfRule type="dataBar" priority="2">
       <dataBar showValue="0">
         <cfvo type="min"/>
-        <cfvo type="num" val="300"/>
+        <cfvo type="max"/>
         <color theme="1" tint="0.249977111117893"/>
       </dataBar>
       <extLst>
@@ -1515,9 +1513,7 @@
           <x14:cfRule type="dataBar" id="{A1CFA2DC-DD05-4F4A-9ED8-061BBFC5526A}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="num">
-                <xm:f>300</xm:f>
-              </x14:cfvo>
+              <x14:cfvo type="autoMax"/>
               <x14:negativeFillColor rgb="FFFF0000"/>
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>

</xml_diff>